<commit_message>
openEHR-EHR-CLUSTER.auscultation-chest.v1.adl: oversatt til norsk. ikke ferdig enda, mangler noe begrep. openEHR-EHR-CLUSTER.exam.v1.adl: oversatt til norsk. openEHR-EHR-CLUSTER.identification_medicine.v1.adl. Ferdigstilt med definisjoner og innhold. Må sjekkes med Kristin og Hilde. openEHR-EHR-CLUSTER.information_source.v1.adl: ferdigstilt. Registrering av informasjonskilde ved allergier. Må sjekkes med Kristin og Hilde. openEHR-EHR-EVALUATION.adverse_reaction_fhir.v1.adl: endret for å passe med norsk standard for kritisk informasjon. Fjernet koder. Meldes inn til godkjenning. openEHR-EHR-EVALUATION.risk.v1.adl: oversatt til norsk. Meldes inn til godkjenning. openEHR-EHR-OBSERVATION.organ_status_evaluation_surgery.v1.adl: ny revisjon med mulighet for å legge til undersøksesfunn. templates/Surgery/Operatørvurdering.v1.oet: aktualisert arketype organstatus kirurgi
</commit_message>
<xml_diff>
--- a/surgery/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/surgery/Arketyper_operasjonsplanlegging_status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="92">
   <si>
     <t>Type</t>
   </si>
@@ -137,9 +137,6 @@
 Må oversettes til engelsk.</t>
   </si>
   <si>
-    <t>Skal den brukes?</t>
-  </si>
-  <si>
     <t>meldt 05.02.15</t>
   </si>
   <si>
@@ -150,7 +147,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Må meldes til godkjenning.</t>
+      <t>Må meldes til godkjenning</t>
     </r>
     <r>
       <rPr>
@@ -160,28 +157,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
+      <t xml:space="preserve">.  ok </t>
     </r>
     <r>
       <rPr>
@@ -197,122 +173,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Oppdatert versjon må importeres og tas i bruk</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Endring må synkroniseres med arketyper.no og sende på e-post til Silje.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- ok, sendt e-post til Silje 09.02</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Må meldes endring. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- ok, sendt e-post til Silje 09.02</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Mangler DIPS endring </t>
     </r>
     <r>
@@ -448,43 +308,337 @@
     <t>NYHA heart failure classification</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Må importeres på nytt når oversettelsen i arketyper.no er godkjent.</t>
-    </r>
-  </si>
-  <si>
     <t>ok. 
 Importert med foreløpig norsk oversettelse.</t>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Vurdering anestesirisiko
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk assessment anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <t>nb
+en</t>
+  </si>
+  <si>
+    <t>godkjent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Planlagt anestesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>planned anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Organstatus evaluering kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>organstatus evaluation surgery</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Risikofaktor hjerte anestesi
+ID: r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isk factor heart anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Risikofaktor lunge anestesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk factor lungs anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spesifikke risikofaktorer anestesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specific risk factors ansthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Annen risikofaktor anesthesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>other risk factors anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Risikofaktor medisiner kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk factor medicine surgery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Medikamenter ved kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>medicine surgery</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spesielle behov kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>special requirements surgery</t>
+    </r>
+  </si>
+  <si>
+    <t>ok i GIT
+klar til intern gjennomgang</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Risikofaktor andre organer anestesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk factor other organs anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <t>Må diskuteres internt og nasjonalt
+Ligger i arketyper.no men passer ikke:(</t>
+  </si>
+  <si>
+    <t>Usikker</t>
+  </si>
+  <si>
+    <t>Overfølsomhetsreaksjoner/Allergier</t>
+  </si>
+  <si>
+    <t>Blodtrykk</t>
+  </si>
+  <si>
+    <t>Må lastes opp i arketyper.no 
+Måoversettes til engelsk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok 
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hastegrad detaljer
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>priority details</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omsorgsnivå
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>care-level</t>
+    </r>
+  </si>
+  <si>
+    <t>Skal ikke meldes til godkjenning, da den kun brukes for å løse et probleme med å kjøre Classic og Arena samtidig. Dermed kun lokal betydning.</t>
+  </si>
+  <si>
+    <t>Skal ikke meldes til godkjenning, brukes kun i påvente av rett bestilling/instruction (behandlingsplan)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Knivtid
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>estimated surgery time</t>
+    </r>
+  </si>
+  <si>
+    <t>Skal ikke meldes til godkjenning. Kun midlertidig. Vil bli en activity i procedure request.</t>
+  </si>
+  <si>
+    <t>Viktig informasjon prosedyre</t>
+  </si>
+  <si>
+    <t>nb
+no</t>
+  </si>
+  <si>
+    <r>
+      <t>Ønsket helsepersonell
+ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required medical personell</t>
+    </r>
+  </si>
+  <si>
+    <t>Health risk</t>
+  </si>
+  <si>
+    <t>ok. Oversatt til norsk.</t>
+  </si>
+  <si>
+    <t>Foreligger kun på engelsk.</t>
+  </si>
+  <si>
+    <t>Ikke godkjent.</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
@@ -501,7 +655,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  ok </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -516,340 +670,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Vurdering anestesirisiko
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>risk assessment anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <t>nb
-en</t>
-  </si>
-  <si>
-    <t>godkjent</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Planlagt anestesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>planned anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Organstatus evaluering kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>organstatus evaluation surgery</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Risikofaktor hjerte anestesi
-ID: r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>isk factor heart anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Risikofaktor lunge anestesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>risk factor lungs anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Spesifikke risikofaktorer anestesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>specific risk factors ansthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Annen risikofaktor anesthesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>other risk factors anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Risikofaktor medisiner kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>risk factor medicine surgery</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Medikamenter ved kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>medicine surgery</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Spesielle behov kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>special requirements surgery</t>
-    </r>
-  </si>
-  <si>
-    <t>ok i GIT
-klar til intern gjennomgang</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Risikofaktor andre organer anestesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>risk factor other organs anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <t>Må diskuteres internt og nasjonalt
-Ligger i arketyper.no men passer ikke:(</t>
-  </si>
-  <si>
-    <t>Usikker</t>
-  </si>
-  <si>
-    <t>Overfølsomhetsreaksjoner/Allergier</t>
-  </si>
-  <si>
-    <t>Blodtrykk</t>
-  </si>
-  <si>
-    <t>Må lastes opp i arketyper.no 
-Måoversettes til engelsk.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ok 
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hastegrad detaljer
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>priority details</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Omsorgsnivå
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>care-level</t>
-    </r>
-  </si>
-  <si>
-    <t>Skal ikke meldes til godkjenning, da den kun brukes for å løse et probleme med å kjøre Classic og Arena samtidig. Dermed kun lokal betydning.</t>
-  </si>
-  <si>
-    <t>Skal ikke meldes til godkjenning, brukes kun i påvente av rett bestilling/instruction (behandlingsplan)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Knivtid
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>estimated surgery time</t>
-    </r>
-  </si>
-  <si>
-    <t>Skal ikke meldes til godkjenning. Kun midlertidig. Vil bli en activity i procedure request.</t>
-  </si>
-  <si>
-    <t>Viktig informasjon prosedyre</t>
-  </si>
-  <si>
-    <t>nb
-no</t>
-  </si>
-  <si>
-    <r>
-      <t>Ønsket helsepersonell
-ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>required medical personell</t>
-    </r>
-  </si>
-  <si>
-    <t>Health risk</t>
-  </si>
-  <si>
-    <t>ok. Oversatt til norsk.</t>
-  </si>
-  <si>
-    <t>Foreligger kun på engelsk.</t>
-  </si>
-  <si>
-    <t>Ikke godkjent.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
+    <t>Må importeres på nytt når oversettelsen i arketyper.no er godkjent.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Må meldes endring. </t>
     </r>
     <r>
       <rPr>
@@ -859,19 +684,44 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Oppdatert versjon må importeres på nytt når oversettelsen er godkjent og tas i bruk.</t>
-    </r>
+      <t>- ok, sendt e-post til Silje 09.02</t>
+    </r>
+  </si>
+  <si>
+    <t>Oppdatert versjon må importeres på nytt når oversettelsen er godkjent og tas i bruk.</t>
+  </si>
+  <si>
+    <t>Oppdatert versjon må importeres og tas i bruk</t>
+  </si>
+  <si>
+    <r>
+      <t>Endring må synkroniseres med arketyper.no og sende på e-post til Silje.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- ok, sendt e-post til Silje 09.02</t>
+    </r>
+  </si>
+  <si>
+    <t>Auscultasjon chest</t>
+  </si>
+  <si>
+    <t>oversatt. Venter på endelig oversettelse fra Tomas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finnes ikke. </t>
+  </si>
+  <si>
+    <t>Må sendes til Silje og meldes til godkjenning.</t>
+  </si>
+  <si>
+    <t>Exam</t>
   </si>
 </sst>
 </file>
@@ -970,7 +820,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1313,13 +1163,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1375,9 +1234,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1408,25 +1264,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1438,9 +1282,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1471,13 +1312,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1486,55 +1321,103 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1819,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1861,14 +1744,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>53</v>
+      <c r="C2" s="65" t="s">
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -1877,305 +1760,345 @@
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="15" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>37</v>
-      </c>
+      <c r="F3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="32"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" s="20" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>20</v>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="E4" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="26" t="s">
+      <c r="E5" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="19" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="15" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>85</v>
+      <c r="B7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="49" t="s">
-        <v>86</v>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="72" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="C10" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
-      <c r="B11" s="48" t="s">
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+      <c r="B13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="44" t="s">
+      <c r="C13" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="F13" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="35"/>
-    </row>
-    <row r="13" spans="1:8" s="8" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="F14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" s="8" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="29" t="s">
+      <c r="C15" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="40" t="s">
+      <c r="B16" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="19" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="55" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="55"/>
+      <c r="G17" s="76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="68"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2193,48 +2116,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="70" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" style="64" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="64" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42" style="64" customWidth="1"/>
-    <col min="7" max="7" width="45.6640625" style="64" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="64"/>
+    <col min="1" max="1" width="11.44140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" style="55" customWidth="1"/>
+    <col min="7" max="7" width="45.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="61" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:7" s="52" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="51" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="54" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>74</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>32</v>
@@ -2243,19 +2166,19 @@
         <v>33</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>32</v>
@@ -2264,19 +2187,19 @@
         <v>33</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>32</v>
@@ -2290,99 +2213,99 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>82</v>
+        <v>42</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="49" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>82</v>
+        <v>43</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>75</v>
-      </c>
-      <c r="C9" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>82</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>33</v>
@@ -2394,58 +2317,58 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="67" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="66"/>
-      <c r="B10" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="29" t="s">
+    <row r="10" spans="1:7" s="58" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="57"/>
+      <c r="B10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="66"/>
-      <c r="B11" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>82</v>
+      <c r="A11" s="57"/>
+      <c r="B11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="71"/>
-      <c r="B12" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="62" t="s">
+      <c r="A12" s="62"/>
+      <c r="B12" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>82</v>
+      <c r="C12" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>33</v>
@@ -2457,39 +2380,39 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="67" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:7" s="58" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="29" t="s">
+      <c r="B13" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>82</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>33</v>
@@ -2502,120 +2425,120 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="29" t="s">
+      <c r="D15" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
+      <c r="B17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="29" t="s">
+      <c r="C17" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F17" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G17" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="29" t="s">
+    <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
+      <c r="B18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F18" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G18" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="29" t="s">
+    <row r="19" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
+      <c r="B19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G19" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>33</v>
@@ -2628,15 +2551,15 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="49" t="s">
-        <v>82</v>
+        <v>51</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>75</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>33</v>
@@ -2649,35 +2572,35 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="68"/>
-      <c r="B22" s="42" t="s">
+      <c r="A22" s="59"/>
+      <c r="B22" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>69</v>
+      <c r="C23" s="40" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
openEHR-EHR-EVALUATION.check_list-medication.v1.adl: rettet noen skrivefeil templates/Surgery/Operatørvurdering.v1.oet: lagt til oppdatert medication list surgery/Arketyper_operasjonsplanlegging_status.xlsx: oppdatert satus etter at arketyper ble meldt inn til godkjenning.
</commit_message>
<xml_diff>
--- a/surgery/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/surgery/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="90">
   <si>
     <t>Type</t>
   </si>
@@ -462,38 +462,6 @@
     <t>Ikke godkjent.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Oppdatert versjon må importeres på nytt når oversettelsen er godkjent og tas i bruk.</t>
-    </r>
-  </si>
-  <si>
     <t>Må importeres på nytt når oversettelsen i arketyper.no er godkjent.</t>
   </si>
   <si>
@@ -585,6 +553,21 @@
   <si>
     <t>Kroppsdel
 ID: Bodypart</t>
+  </si>
+  <si>
+    <t>Check list medicine</t>
+  </si>
+  <si>
+    <t>Redigeres for tiden</t>
+  </si>
+  <si>
+    <t>Oversatt og endringer foreslått. Må diskuteres internt</t>
+  </si>
+  <si>
+    <t>meldt 07.03.15 med oversettelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meldt 07.03.15 </t>
   </si>
 </sst>
 </file>
@@ -651,7 +634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,6 +650,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -939,13 +928,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1230,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,7 +1283,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H2" s="27"/>
     </row>
@@ -1322,7 +1314,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>15</v>
@@ -1331,11 +1323,11 @@
         <v>18</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -1359,7 +1351,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1403,7 +1395,7 @@
         <v>33</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1423,18 +1415,18 @@
         <v>63</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>62</v>
@@ -1446,83 +1438,85 @@
         <v>63</v>
       </c>
       <c r="F9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="G11" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="7"/>
+      <c r="F12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
+      <c r="A13" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>37</v>
@@ -1541,7 +1535,7 @@
     <row r="14" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>37</v>
@@ -1557,9 +1551,10 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>37</v>
@@ -1573,86 +1568,104 @@
       <c r="F15" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="28"/>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
-        <v>23</v>
-      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C18" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="F18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E19" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="25"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1664,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,25 +1694,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="19" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1723,7 +1736,7 @@
         <v>55</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1744,7 +1757,7 @@
         <v>58</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1763,7 +1776,7 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1784,7 +1797,7 @@
         <v>56</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1805,7 +1818,7 @@
         <v>56</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1826,7 +1839,7 @@
         <v>56</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1847,7 +1860,7 @@
         <v>56</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1868,7 +1881,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1889,7 +1902,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1910,13 +1923,13 @@
         <v>56</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>52</v>
@@ -1931,13 +1944,13 @@
         <v>14</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>15</v>
@@ -1949,16 +1962,16 @@
         <v>32</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>15</v>
@@ -1970,16 +1983,16 @@
         <v>32</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>15</v>
@@ -1994,7 +2007,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2017,7 +2030,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2038,13 +2051,13 @@
         <v>14</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>52</v>
@@ -2059,7 +2072,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
templates/Surgery/Oppsummering.oet: lagt til tilleggsprosedyre
</commit_message>
<xml_diff>
--- a/surgery/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/surgery/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="89">
   <si>
     <t>Type</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Oversettelse til norsk klar men ikke godkjent</t>
   </si>
   <si>
-    <t>Ikke godkjent</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
   </si>
   <si>
     <t>nb</t>
-  </si>
-  <si>
-    <t>Ikke lastet opp</t>
   </si>
   <si>
     <t>meldt 05.02.15</t>
@@ -429,10 +423,6 @@
     <t>Skal ikke meldes til godkjenning. Kun midlertidig. Vil bli en activity i procedure request.</t>
   </si>
   <si>
-    <t>nb
-no</t>
-  </si>
-  <si>
     <r>
       <t>Ønsket helsepersonell
 ID:</t>
@@ -459,9 +449,6 @@
     <t>Foreligger kun på engelsk.</t>
   </si>
   <si>
-    <t>Ikke godkjent.</t>
-  </si>
-  <si>
     <t>Må importeres på nytt når oversettelsen i arketyper.no er godkjent.</t>
   </si>
   <si>
@@ -511,12 +498,6 @@
 ID: properative evaluation anesthesia</t>
   </si>
   <si>
-    <t>Adverse reaction FHIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finnes kun på engelsk. </t>
-  </si>
-  <si>
     <t>Viktig informasjon prosedyre
 ID: important information procedure</t>
   </si>
@@ -529,19 +510,7 @@
 ID: preopertaive clarifications</t>
   </si>
   <si>
-    <t>Må lastes opp i arketyper.no 
-Må oversettes til engelsk?</t>
-  </si>
-  <si>
-    <t>Skal ikke meldes til godkjenning, brukes kun i påvente av rett bestilling/instruction</t>
-  </si>
-  <si>
     <t xml:space="preserve">Skal ikke meldes til godkjenning, brukes kun i påvente av rett bestilling/instruction </t>
-  </si>
-  <si>
-    <t>Må lastes opp i arketyper.no 
-Må meldes til godkjenning
-Må oversettes til engelsk.</t>
   </si>
   <si>
     <t>Check list</t>
@@ -561,13 +530,38 @@
     <t>Redigeres for tiden</t>
   </si>
   <si>
-    <t>Oversatt og endringer foreslått. Må diskuteres internt</t>
-  </si>
-  <si>
     <t>meldt 07.03.15 med oversettelse</t>
   </si>
   <si>
     <t xml:space="preserve">meldt 07.03.15 </t>
+  </si>
+  <si>
+    <t>Meldt 10.03</t>
+  </si>
+  <si>
+    <t>Må oversettes til engelsk.</t>
+  </si>
+  <si>
+    <t>Meldt 10.03.15</t>
+  </si>
+  <si>
+    <t>OK. Inkubator: operasjonsplanlegging</t>
+  </si>
+  <si>
+    <t>OK. Inkubator: innkomstjournal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb
+</t>
+  </si>
+  <si>
+    <t>Skal ikke meldes til godkjenning, brukes kun i påvente av at action tas i bruk.</t>
+  </si>
+  <si>
+    <t>meldt 10.03.15</t>
+  </si>
+  <si>
+    <t>Må oversettes til engelsk?</t>
   </si>
 </sst>
 </file>
@@ -886,15 +880,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -928,9 +913,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -938,6 +920,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1222,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,25 +1235,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1270,22 +1264,22 @@
       <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>45</v>
+      <c r="C2" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="27"/>
+        <v>61</v>
+      </c>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" s="9" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
@@ -1294,378 +1288,357 @@
       <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="C6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>45</v>
+      <c r="C7" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>21</v>
+      <c r="A8" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>21</v>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>87</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>74</v>
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>23</v>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>68</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="28"/>
       <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>37</v>
+      <c r="C13" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="32" t="s">
-        <v>37</v>
+      <c r="C14" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="28"/>
-    </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="C18" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="F18" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="22"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1677,401 +1650,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42" style="20" customWidth="1"/>
-    <col min="7" max="7" width="45.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="20"/>
+    <col min="1" max="1" width="11.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" style="19" customWidth="1"/>
+    <col min="7" max="7" width="45.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="19" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:7" s="34" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="35"/>
+      <c r="B3" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="35"/>
+      <c r="B4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="35"/>
+      <c r="B6" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="35"/>
+      <c r="B8" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="7" t="s">
+      <c r="C8" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="G8" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="36" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="35"/>
+      <c r="B10" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+      <c r="B11" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+      <c r="B12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+      <c r="B13" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+      <c r="B14" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
+      <c r="B15" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="36" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="C16" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="7" t="s">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="35"/>
+      <c r="B17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="7" t="s">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="35"/>
+      <c r="B18" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="7" t="s">
+      <c r="D18" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="29" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
opt/Surgery/Beslutningsnotat.v6.opt: gjort tilleggsprosedyre i action arketypen mandatory opt/Surgery/Operatørvurdering v3.opt: gjort tilleggsprosedyre i action arketypen mandatory templates/SurgeryProsedyre.oet: gjort tilleggsprosedyre mandatory
</commit_message>
<xml_diff>
--- a/surgery/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/surgery/Arketyper_operasjonsplanlegging_status.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="124">
   <si>
     <t>Type</t>
   </si>
@@ -361,9 +361,6 @@
   </si>
   <si>
     <t>Citation/sitering v1</t>
-  </si>
-  <si>
-    <t>NYHA klassifikasjon</t>
   </si>
   <si>
     <t>Ny versjon med små justeringer 14. august. Ikke lastet opp i vår ckm og ikke tatt i bruk. Avventer at høringer er gjennomført.</t>
@@ -672,6 +669,12 @@
   </si>
   <si>
     <t>Brukes ikke lenger. Aenstesi ny modellert med procedure som utgangspunkt.</t>
+  </si>
+  <si>
+    <t>NYHA klassifikasjon v1</t>
+  </si>
+  <si>
+    <t>Endret til v0 nasjonalt (2.09.15). Denne endringen er ikke tatt inn.</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1038,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1213,6 +1216,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1501,7 +1507,7 @@
   <dimension ref="A1:BI20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,10 +2051,10 @@
         <v>67</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>10</v>
+        <v>122</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>123</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>11</v>
@@ -2057,7 +2063,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
@@ -2120,7 +2126,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>10</v>
@@ -2129,10 +2135,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="39" t="s">
         <v>84</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>85</v>
       </c>
       <c r="G9" s="41"/>
       <c r="H9" s="41"/>
@@ -2207,7 +2213,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2270,16 +2276,16 @@
         <v>68</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>65</v>
@@ -2302,7 +2308,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2763,7 +2769,7 @@
         <v>78</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>11</v>
@@ -2965,7 +2971,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>19</v>
@@ -3063,7 +3069,7 @@
         <v>67</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>19</v>
@@ -3075,7 +3081,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -3161,7 +3167,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>19</v>
@@ -3173,7 +3179,7 @@
         <v>33</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -3259,7 +3265,7 @@
         <v>67</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>19</v>
@@ -3271,7 +3277,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -3357,7 +3363,7 @@
         <v>67</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>19</v>
@@ -3369,7 +3375,7 @@
         <v>33</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -3455,7 +3461,7 @@
         <v>67</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>19</v>
@@ -3467,7 +3473,7 @@
         <v>33</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -3553,7 +3559,7 @@
         <v>67</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>19</v>
@@ -3565,7 +3571,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -3651,7 +3657,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>19</v>
@@ -3749,7 +3755,7 @@
         <v>67</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>10</v>
@@ -3761,7 +3767,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -3847,7 +3853,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>19</v>
@@ -3859,7 +3865,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -3945,7 +3951,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>19</v>
@@ -3957,7 +3963,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -4043,19 +4049,19 @@
         <v>67</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -4141,7 +4147,7 @@
         <v>67</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>10</v>
@@ -4150,10 +4156,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -4239,7 +4245,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>10</v>
@@ -4248,10 +4254,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -4426,10 +4432,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
@@ -4800,10 +4806,10 @@
         <v>67</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="37" t="s">
         <v>34</v>
@@ -4812,7 +4818,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4820,7 +4826,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>43</v>
@@ -4900,7 +4906,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>43</v>
@@ -4912,7 +4918,7 @@
         <v>45</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4920,7 +4926,7 @@
         <v>70</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>43</v>
@@ -4943,7 +4949,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="37" t="s">
         <v>34</v>
@@ -4963,7 +4969,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="50" t="s">
         <v>13</v>
@@ -4983,7 +4989,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Lastet opp oppdaterte filer fra nasjinal IKT Fjernet v1 arketyper hvor jeg lastet opp nye med versjon 0 Laget nye arketyper for innkomstjournal
</commit_message>
<xml_diff>
--- a/surgery/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/surgery/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="5655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -738,7 +738,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +760,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1035,7 +1041,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1216,6 +1222,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1507,18 +1519,18 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="21.33203125" style="2"/>
+    <col min="6" max="6" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="21.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1605,7 @@
       <c r="BH1" s="25"/>
       <c r="BI1" s="25"/>
     </row>
-    <row r="2" spans="1:61" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>67</v>
       </c>
@@ -1668,7 +1680,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
     </row>
-    <row r="3" spans="1:61" s="9" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:61" s="9" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>67</v>
       </c>
@@ -1743,7 +1755,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="2"/>
     </row>
-    <row r="4" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:61" s="42" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>67</v>
       </c>
@@ -1818,7 +1830,7 @@
       <c r="BH4" s="41"/>
       <c r="BI4" s="41"/>
     </row>
-    <row r="5" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:61" s="42" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="40" t="s">
         <v>67</v>
       </c>
@@ -1893,7 +1905,7 @@
       <c r="BH5" s="41"/>
       <c r="BI5" s="41"/>
     </row>
-    <row r="6" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:61" s="42" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>67</v>
       </c>
@@ -1968,7 +1980,7 @@
       <c r="BH6" s="41"/>
       <c r="BI6" s="41"/>
     </row>
-    <row r="7" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:61" s="42" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="40" t="s">
         <v>67</v>
       </c>
@@ -2043,7 +2055,7 @@
       <c r="BH7" s="41"/>
       <c r="BI7" s="41"/>
     </row>
-    <row r="8" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:61" s="42" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="s">
         <v>67</v>
       </c>
@@ -2118,7 +2130,7 @@
       <c r="BH8" s="41"/>
       <c r="BI8" s="41"/>
     </row>
-    <row r="9" spans="1:61" s="42" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:61" s="42" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
         <v>67</v>
       </c>
@@ -2193,7 +2205,7 @@
       <c r="BH9" s="41"/>
       <c r="BI9" s="41"/>
     </row>
-    <row r="10" spans="1:61" s="10" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:61" s="10" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>68</v>
       </c>
@@ -2268,7 +2280,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="2"/>
     </row>
-    <row r="11" spans="1:61" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>68</v>
       </c>
@@ -2288,7 +2300,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:61" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>69</v>
       </c>
@@ -2363,7 +2375,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="2"/>
     </row>
-    <row r="13" spans="1:61" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>70</v>
       </c>
@@ -2438,7 +2450,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="2"/>
     </row>
-    <row r="14" spans="1:61" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>70</v>
       </c>
@@ -2513,7 +2525,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="2"/>
     </row>
-    <row r="15" spans="1:61" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>70</v>
       </c>
@@ -2588,7 +2600,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="2"/>
     </row>
-    <row r="16" spans="1:61" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>70</v>
       </c>
@@ -2663,7 +2675,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="2"/>
     </row>
-    <row r="17" spans="1:61" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:61" s="6" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36" t="s">
         <v>70</v>
       </c>
@@ -2738,7 +2750,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="2"/>
     </row>
-    <row r="18" spans="1:61" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:61" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
         <v>70</v>
       </c>
@@ -2758,7 +2770,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:61" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:61" s="10" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>6</v>
       </c>
@@ -2833,7 +2845,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="2"/>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="55"/>
       <c r="C20" s="56"/>
       <c r="D20" s="57"/>
@@ -2851,21 +2863,21 @@
   <dimension ref="A1:CF18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="12"/>
+    <col min="7" max="16384" width="11.5703125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" s="16" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:84" s="16" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2963,11 +2975,11 @@
       <c r="CE1" s="18"/>
       <c r="CF1" s="18"/>
     </row>
-    <row r="2" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="63" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2979,7 +2991,7 @@
       <c r="E2" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="62" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="19"/>
@@ -3061,11 +3073,11 @@
       <c r="CE2" s="19"/>
       <c r="CF2" s="19"/>
     </row>
-    <row r="3" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="63" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -3077,7 +3089,7 @@
       <c r="E3" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="62" t="s">
         <v>89</v>
       </c>
       <c r="G3" s="19"/>
@@ -3159,7 +3171,7 @@
       <c r="CE3" s="19"/>
       <c r="CF3" s="19"/>
     </row>
-    <row r="4" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>67</v>
       </c>
@@ -3257,7 +3269,7 @@
       <c r="CE4" s="19"/>
       <c r="CF4" s="19"/>
     </row>
-    <row r="5" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>67</v>
       </c>
@@ -3355,11 +3367,11 @@
       <c r="CE5" s="19"/>
       <c r="CF5" s="19"/>
     </row>
-    <row r="6" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="63" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -3371,7 +3383,7 @@
       <c r="E6" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="62" t="s">
         <v>91</v>
       </c>
       <c r="G6" s="19"/>
@@ -3453,11 +3465,11 @@
       <c r="CE6" s="19"/>
       <c r="CF6" s="19"/>
     </row>
-    <row r="7" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="63" t="s">
         <v>101</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -3469,7 +3481,7 @@
       <c r="E7" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="62" t="s">
         <v>91</v>
       </c>
       <c r="G7" s="19"/>
@@ -3551,7 +3563,7 @@
       <c r="CE7" s="19"/>
       <c r="CF7" s="19"/>
     </row>
-    <row r="8" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>67</v>
       </c>
@@ -3649,11 +3661,11 @@
       <c r="CE8" s="19"/>
       <c r="CF8" s="19"/>
     </row>
-    <row r="9" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="63" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -3665,7 +3677,7 @@
       <c r="E9" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="62" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="19"/>
@@ -3747,7 +3759,7 @@
       <c r="CE9" s="19"/>
       <c r="CF9" s="19"/>
     </row>
-    <row r="10" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>67</v>
       </c>
@@ -3845,7 +3857,7 @@
       <c r="CE10" s="19"/>
       <c r="CF10" s="19"/>
     </row>
-    <row r="11" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>67</v>
       </c>
@@ -3943,7 +3955,7 @@
       <c r="CE11" s="19"/>
       <c r="CF11" s="19"/>
     </row>
-    <row r="12" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>67</v>
       </c>
@@ -4041,7 +4053,7 @@
       <c r="CE12" s="19"/>
       <c r="CF12" s="19"/>
     </row>
-    <row r="13" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>67</v>
       </c>
@@ -4139,7 +4151,7 @@
       <c r="CE13" s="19"/>
       <c r="CF13" s="19"/>
     </row>
-    <row r="14" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>67</v>
       </c>
@@ -4237,7 +4249,7 @@
       <c r="CE14" s="19"/>
       <c r="CF14" s="19"/>
     </row>
-    <row r="15" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>70</v>
       </c>
@@ -4335,7 +4347,7 @@
       <c r="CE15" s="19"/>
       <c r="CF15" s="19"/>
     </row>
-    <row r="16" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="E16" s="15" t="s">
         <v>122</v>
       </c>
@@ -4418,7 +4430,7 @@
       <c r="CE16" s="19"/>
       <c r="CF16" s="19"/>
     </row>
-    <row r="17" spans="1:84" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
         <v>70</v>
       </c>
@@ -4516,7 +4528,7 @@
       <c r="CE17" s="19"/>
       <c r="CF17" s="19"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.25">
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -4610,18 +4622,18 @@
       <selection activeCell="A2" sqref="A2:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" style="47" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" style="47" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="47" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="47"/>
+    <col min="1" max="1" width="13.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="47" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" style="47" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -4641,7 +4653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>67</v>
       </c>
@@ -4661,7 +4673,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>69</v>
       </c>
@@ -4681,7 +4693,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>69</v>
       </c>
@@ -4701,7 +4713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>69</v>
       </c>
@@ -4721,7 +4733,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>69</v>
       </c>
@@ -4741,7 +4753,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>70</v>
       </c>
@@ -4761,7 +4773,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>70</v>
       </c>
@@ -4781,7 +4793,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>70</v>
       </c>
@@ -4801,7 +4813,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>67</v>
       </c>
@@ -4821,7 +4833,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>67</v>
       </c>
@@ -4841,7 +4853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>67</v>
       </c>
@@ -4861,7 +4873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>67</v>
       </c>
@@ -4881,7 +4893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>67</v>
       </c>
@@ -4901,7 +4913,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>70</v>
       </c>
@@ -4921,7 +4933,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>70</v>
       </c>
@@ -4941,7 +4953,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>70</v>
       </c>
@@ -4961,7 +4973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
         <v>70</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>70</v>
       </c>

</xml_diff>